<commit_message>
Test command file + optimization
optimized scrim function
optimized removescrim funciton
added testing file
</commit_message>
<xml_diff>
--- a/scrimrole.xlsx
+++ b/scrimrole.xlsx
@@ -52,6 +52,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1347,13 +1415,7 @@
     <row r="996"/>
     <row r="997"/>
     <row r="998"/>
-    <row r="999">
-      <c r="A999" t="inlineStr">
-        <is>
-          <t>marley-EE#7068</t>
-        </is>
-      </c>
-    </row>
+    <row r="999"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>